<commit_message>
Updated Scrumsheet for completed Customer Class
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Desktop\cse1325\P05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1D1EA50-BF5B-47A8-AF30-84C412454BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638179A2-C086-457B-ABF4-CCA16162398F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="142">
   <si>
     <t>Product Name:</t>
   </si>
@@ -462,6 +462,12 @@
   </si>
   <si>
     <t>Add Customer to Github with build.xml file</t>
+  </si>
+  <si>
+    <t>Finished in Sprint 1</t>
+  </si>
+  <si>
+    <t>Completed Day 2</t>
   </si>
 </sst>
 </file>
@@ -963,19 +969,19 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>17</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1266,22 +1272,22 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3060,7 +3066,7 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>1905480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>125002</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3637,7 +3643,7 @@
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
     <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3837,11 +3843,11 @@
       </c>
       <c r="B13" s="5">
         <f>B12-C13</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 1")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5"/>
@@ -3861,7 +3867,7 @@
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 2")</f>
@@ -3885,7 +3891,7 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 3")</f>
@@ -3909,7 +3915,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -3929,7 +3935,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -4060,9 +4066,11 @@
       <c r="E24" s="16">
         <v>3</v>
       </c>
-      <c r="F24" s="17"/>
+      <c r="F24" s="17">
+        <v>1</v>
+      </c>
       <c r="G24" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H24" s="18" t="s">
         <v>31</v>
@@ -4091,7 +4099,9 @@
       <c r="E25" s="16">
         <v>3</v>
       </c>
-      <c r="F25" s="17"/>
+      <c r="F25" s="17">
+        <v>1</v>
+      </c>
       <c r="G25" s="17" t="s">
         <v>136</v>
       </c>
@@ -4122,7 +4132,9 @@
       <c r="E26" s="16">
         <v>8</v>
       </c>
-      <c r="F26" s="17"/>
+      <c r="F26" s="17">
+        <v>1</v>
+      </c>
       <c r="G26" s="17" t="s">
         <v>136</v>
       </c>
@@ -4151,7 +4163,9 @@
       <c r="E27" s="16">
         <v>8</v>
       </c>
-      <c r="F27" s="17"/>
+      <c r="F27" s="17">
+        <v>1</v>
+      </c>
       <c r="G27" s="17" t="s">
         <v>136</v>
       </c>
@@ -4180,7 +4194,9 @@
       <c r="E28" s="16">
         <v>13</v>
       </c>
-      <c r="F28" s="17"/>
+      <c r="F28" s="17">
+        <v>1</v>
+      </c>
       <c r="G28" s="17" t="s">
         <v>136</v>
       </c>
@@ -5378,8 +5394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5515,11 +5531,11 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D9" s="25"/>
       <c r="E9" s="25"/>
@@ -5533,7 +5549,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5551,7 +5567,7 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
@@ -5569,7 +5585,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5587,7 +5603,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5605,7 +5621,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5670,7 +5686,9 @@
       <c r="D18" s="39" t="s">
         <v>137</v>
       </c>
-      <c r="E18" s="37"/>
+      <c r="E18" s="37" t="s">
+        <v>141</v>
+      </c>
       <c r="F18" s="38"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -5684,7 +5702,9 @@
       <c r="D19" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="E19" s="37"/>
+      <c r="E19" s="37" t="s">
+        <v>141</v>
+      </c>
       <c r="F19" s="38"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
@@ -5698,7 +5718,9 @@
       <c r="D20" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="E20" s="37"/>
+      <c r="E20" s="37" t="s">
+        <v>141</v>
+      </c>
       <c r="F20" s="38"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Updated scrum file for finished Customer
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Desktop\cse1325\P05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{638179A2-C086-457B-ABF4-CCA16162398F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4431E0FA-49FA-4747-8B42-11BBACA66C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="149">
   <si>
     <t>Product Name:</t>
   </si>
@@ -468,6 +468,27 @@
   </si>
   <si>
     <t>Completed Day 2</t>
+  </si>
+  <si>
+    <t>Write Option class</t>
+  </si>
+  <si>
+    <t>Build and test option</t>
+  </si>
+  <si>
+    <t>Add Option to Github</t>
+  </si>
+  <si>
+    <t>Completed Day 3</t>
+  </si>
+  <si>
+    <t>Ryan Harris</t>
+  </si>
+  <si>
+    <t>WEBUILDPCS</t>
+  </si>
+  <si>
+    <t>R.H</t>
   </si>
 </sst>
 </file>
@@ -622,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -746,6 +767,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -969,19 +993,19 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>16</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1266,13 +1290,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -3642,8 +3666,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3666,7 +3690,9 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43"/>
+      <c r="B1" s="43" t="s">
+        <v>146</v>
+      </c>
       <c r="C1" s="43"/>
       <c r="D1" s="43"/>
       <c r="E1" s="43"/>
@@ -3682,7 +3708,9 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="44"/>
+      <c r="B2" s="44" t="s">
+        <v>147</v>
+      </c>
       <c r="C2" s="44"/>
       <c r="D2" s="44"/>
       <c r="E2" s="44"/>
@@ -3726,14 +3754,20 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="45"/>
+      <c r="B5" s="45" t="s">
+        <v>146</v>
+      </c>
       <c r="C5" s="45"/>
       <c r="D5" s="45"/>
       <c r="E5" s="45"/>
       <c r="F5" s="45"/>
       <c r="G5" s="45"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
+      <c r="H5" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I5" s="46">
+        <v>1002004373</v>
+      </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" s="7" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
@@ -3843,11 +3877,11 @@
       </c>
       <c r="B13" s="5">
         <f>B12-C13</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 1")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5"/>
@@ -3867,7 +3901,7 @@
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 2")</f>
@@ -3891,7 +3925,7 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 3")</f>
@@ -3915,7 +3949,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -3935,7 +3969,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -4103,7 +4137,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
@@ -5394,8 +5428,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView topLeftCell="B9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5498,7 +5532,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5513,7 +5547,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5531,7 +5565,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5553,7 +5587,7 @@
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -5727,30 +5761,48 @@
       <c r="A21" s="4">
         <v>5</v>
       </c>
-      <c r="B21" s="35"/>
+      <c r="B21" s="35" t="s">
+        <v>35</v>
+      </c>
       <c r="C21" s="4"/>
-      <c r="D21" s="39"/>
-      <c r="E21" s="37"/>
+      <c r="D21" s="39" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="F21" s="38"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>6</v>
       </c>
-      <c r="B22" s="35"/>
+      <c r="B22" s="35" t="s">
+        <v>35</v>
+      </c>
       <c r="C22" s="4"/>
-      <c r="D22" s="39"/>
-      <c r="E22" s="37"/>
+      <c r="D22" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E22" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="F22" s="38"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>7</v>
       </c>
-      <c r="B23" s="35"/>
+      <c r="B23" s="35" t="s">
+        <v>35</v>
+      </c>
       <c r="C23" s="4"/>
-      <c r="D23" s="39"/>
-      <c r="E23" s="37"/>
+      <c r="D23" s="39" t="s">
+        <v>144</v>
+      </c>
+      <c r="E23" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="F23" s="38"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Adding updated scrum file for completed Computer class
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Desktop\cse1325\P05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4431E0FA-49FA-4747-8B42-11BBACA66C8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33632D1-C66B-4F14-9E27-FC3CD7AE2865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="152">
   <si>
     <t>Product Name:</t>
   </si>
@@ -489,6 +489,15 @@
   </si>
   <si>
     <t>R.H</t>
+  </si>
+  <si>
+    <t>Write the Computer class</t>
+  </si>
+  <si>
+    <t>Build and test Computer</t>
+  </si>
+  <si>
+    <t>Add Computer to Github</t>
   </si>
 </sst>
 </file>
@@ -753,6 +762,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -767,9 +779,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -993,19 +1002,19 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1290,13 +1299,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>1</c:v>
@@ -3666,8 +3675,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3690,14 +3699,14 @@
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="B1" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="C1" s="43"/>
-      <c r="D1" s="43"/>
-      <c r="E1" s="43"/>
-      <c r="F1" s="43"/>
-      <c r="G1" s="43"/>
+      <c r="C1" s="44"/>
+      <c r="D1" s="44"/>
+      <c r="E1" s="44"/>
+      <c r="F1" s="44"/>
+      <c r="G1" s="44"/>
       <c r="H1" s="5"/>
       <c r="I1" s="6" t="s">
         <v>1</v>
@@ -3708,14 +3717,14 @@
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="44" t="s">
+      <c r="B2" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
       <c r="H2" s="5"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
@@ -3754,66 +3763,66 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="45" t="s">
+      <c r="B5" s="46" t="s">
         <v>146</v>
       </c>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
+      <c r="C5" s="46"/>
+      <c r="D5" s="46"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
+      <c r="G5" s="46"/>
       <c r="H5" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="I5" s="46">
+      <c r="I5" s="41">
         <v>1002004373</v>
       </c>
       <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:10" s="7" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A6"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="41"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
-      <c r="G6" s="41"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
       <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" s="7" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A7"/>
-      <c r="B7" s="41"/>
-      <c r="C7" s="41"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="41"/>
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
       <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" s="7" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A8"/>
-      <c r="B8" s="41"/>
-      <c r="C8" s="41"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
-      <c r="G8" s="41"/>
+      <c r="B8" s="42"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" s="7" customFormat="1" ht="13.15" x14ac:dyDescent="0.35">
       <c r="A9"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
+      <c r="B9" s="42"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9" s="5"/>
@@ -3877,11 +3886,11 @@
       </c>
       <c r="B13" s="5">
         <f>B12-C13</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 1")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5"/>
@@ -3901,7 +3910,7 @@
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 2")</f>
@@ -3925,7 +3934,7 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 3")</f>
@@ -3949,7 +3958,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -3969,7 +3978,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -4041,10 +4050,10 @@
       <c r="C22" s="13"/>
       <c r="D22" s="13"/>
       <c r="E22" s="13"/>
-      <c r="F22" s="42" t="s">
+      <c r="F22" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G22" s="42"/>
+      <c r="G22" s="43"/>
       <c r="H22" s="13"/>
       <c r="I22" s="13" t="s">
         <v>19</v>
@@ -4170,7 +4179,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
       <c r="H26" s="18" t="s">
         <v>31</v>
@@ -5428,8 +5437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView topLeftCell="B6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5532,7 +5541,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5547,7 +5556,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5565,7 +5574,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5587,7 +5596,7 @@
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D10" s="25"/>
       <c r="E10" s="25"/>
@@ -5809,30 +5818,48 @@
       <c r="A24" s="4">
         <v>8</v>
       </c>
-      <c r="B24" s="35"/>
+      <c r="B24" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C24" s="4"/>
-      <c r="D24" s="39"/>
-      <c r="E24" s="37"/>
+      <c r="D24" s="39" t="s">
+        <v>149</v>
+      </c>
+      <c r="E24" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="F24" s="38"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>9</v>
       </c>
-      <c r="B25" s="35"/>
+      <c r="B25" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C25" s="4"/>
-      <c r="D25" s="39"/>
-      <c r="E25" s="37"/>
+      <c r="D25" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="F25" s="38"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>10</v>
       </c>
-      <c r="B26" s="35"/>
+      <c r="B26" s="35" t="s">
+        <v>40</v>
+      </c>
       <c r="C26" s="4"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="37"/>
+      <c r="D26" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E26" s="37" t="s">
+        <v>145</v>
+      </c>
       <c r="F26" s="38"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Finished Scrum file for Sprint 1
</commit_message>
<xml_diff>
--- a/P05/Scrum_ELSA_Sprint_1.xlsx
+++ b/P05/Scrum_ELSA_Sprint_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ryant\Desktop\cse1325\P05\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C33632D1-C66B-4F14-9E27-FC3CD7AE2865}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1491AC87-BFFB-4E73-B452-BF468E9C439A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="158">
   <si>
     <t>Product Name:</t>
   </si>
@@ -452,9 +452,6 @@
     <t>NOTE: This sprint is entirely OPTIONAL – no points will be lost if you ignore it</t>
   </si>
   <si>
-    <t>Not Started</t>
-  </si>
-  <si>
     <t>Write Customer class</t>
   </si>
   <si>
@@ -498,6 +495,27 @@
   </si>
   <si>
     <t>Add Computer to Github</t>
+  </si>
+  <si>
+    <t>Write Order class</t>
+  </si>
+  <si>
+    <t>Build and test Order</t>
+  </si>
+  <si>
+    <t>Add Order to GitHub</t>
+  </si>
+  <si>
+    <t>Completed Day 4</t>
+  </si>
+  <si>
+    <t>Test other classes with Store</t>
+  </si>
+  <si>
+    <t>Add Store to local Repository</t>
+  </si>
+  <si>
+    <t>Add Store to Github</t>
   </si>
 </sst>
 </file>
@@ -1002,19 +1020,19 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>14</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1299,28 +1317,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3675,8 +3693,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -3700,7 +3718,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="44" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C1" s="44"/>
       <c r="D1" s="44"/>
@@ -3718,7 +3736,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="45" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C2" s="45"/>
       <c r="D2" s="45"/>
@@ -3764,7 +3782,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C5" s="46"/>
       <c r="D5" s="46"/>
@@ -3772,7 +3790,7 @@
       <c r="F5" s="46"/>
       <c r="G5" s="46"/>
       <c r="H5" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="I5" s="41">
         <v>1002004373</v>
@@ -3886,11 +3904,11 @@
       </c>
       <c r="B13" s="5">
         <f>B12-C13</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C13" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 1")</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D13" s="9"/>
       <c r="E13" s="5"/>
@@ -3910,7 +3928,7 @@
       </c>
       <c r="B14" s="5">
         <f>B13-C14</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C14" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 2")</f>
@@ -3934,7 +3952,7 @@
       </c>
       <c r="B15" s="5">
         <f>B14-C15</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C15" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 3")</f>
@@ -3958,7 +3976,7 @@
       </c>
       <c r="B16" s="5">
         <f>B15-C16</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -3978,7 +3996,7 @@
       </c>
       <c r="B17" s="5">
         <f>B16-C17</f>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C17" s="9">
         <f>COUNTIF(G$24:G$100,"Finished in Sprint 4")</f>
@@ -4113,7 +4131,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H24" s="18" t="s">
         <v>31</v>
@@ -4146,7 +4164,7 @@
         <v>1</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H25" s="18" t="s">
         <v>36</v>
@@ -4179,7 +4197,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H26" s="18" t="s">
         <v>31</v>
@@ -4210,7 +4228,7 @@
         <v>1</v>
       </c>
       <c r="G27" s="17" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H27" s="18" t="s">
         <v>31</v>
@@ -4241,7 +4259,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="17" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="H28" s="18" t="s">
         <v>31</v>
@@ -5437,8 +5455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AMJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="B6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" topLeftCell="B12" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.59765625" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
@@ -5541,7 +5559,7 @@
       </c>
       <c r="B7" s="25">
         <f>COUNTA(D17:D995)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
@@ -5556,7 +5574,7 @@
       </c>
       <c r="B8" s="25">
         <f t="shared" ref="B8:B14" si="0">B7-C8</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C8" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 1")</f>
@@ -5574,7 +5592,7 @@
       </c>
       <c r="B9" s="25">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C9" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 2")</f>
@@ -5592,7 +5610,7 @@
       </c>
       <c r="B10" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C10" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 3")</f>
@@ -5610,11 +5628,11 @@
       </c>
       <c r="B11" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C11" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 4")</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
@@ -5628,7 +5646,7 @@
       </c>
       <c r="B12" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C12" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 5")</f>
@@ -5646,7 +5664,7 @@
       </c>
       <c r="B13" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C13" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 6")</f>
@@ -5664,7 +5682,7 @@
       </c>
       <c r="B14" s="25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C14" s="25">
         <f>COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5712,9 +5730,7 @@
       </c>
       <c r="B17" s="35"/>
       <c r="C17" s="4"/>
-      <c r="D17" s="36" t="s">
-        <v>132</v>
-      </c>
+      <c r="D17" s="36"/>
       <c r="E17" s="37"/>
       <c r="F17" s="38"/>
     </row>
@@ -5727,10 +5743,10 @@
       </c>
       <c r="C18" s="4"/>
       <c r="D18" s="39" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E18" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F18" s="38"/>
     </row>
@@ -5743,10 +5759,10 @@
       </c>
       <c r="C19" s="4"/>
       <c r="D19" s="39" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E19" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F19" s="38"/>
     </row>
@@ -5759,10 +5775,10 @@
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E20" s="37" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20" s="38"/>
     </row>
@@ -5775,10 +5791,10 @@
       </c>
       <c r="C21" s="4"/>
       <c r="D21" s="39" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E21" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F21" s="38"/>
     </row>
@@ -5791,10 +5807,10 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="39" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E22" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F22" s="38"/>
     </row>
@@ -5807,10 +5823,10 @@
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="39" t="s">
+        <v>143</v>
+      </c>
+      <c r="E23" s="37" t="s">
         <v>144</v>
-      </c>
-      <c r="E23" s="37" t="s">
-        <v>145</v>
       </c>
       <c r="F23" s="38"/>
     </row>
@@ -5823,10 +5839,10 @@
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="39" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E24" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F24" s="38"/>
     </row>
@@ -5839,10 +5855,10 @@
       </c>
       <c r="C25" s="4"/>
       <c r="D25" s="39" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E25" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F25" s="38"/>
     </row>
@@ -5855,10 +5871,10 @@
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="39" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E26" s="37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F26" s="38"/>
     </row>
@@ -5866,60 +5882,96 @@
       <c r="A27" s="4">
         <v>11</v>
       </c>
-      <c r="B27" s="35"/>
+      <c r="B27" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="C27" s="4"/>
-      <c r="D27" s="39"/>
-      <c r="E27" s="37"/>
+      <c r="D27" s="39" t="s">
+        <v>151</v>
+      </c>
+      <c r="E27" s="37" t="s">
+        <v>154</v>
+      </c>
       <c r="F27" s="38"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>12</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="C28" s="4"/>
-      <c r="D28" s="39"/>
-      <c r="E28" s="37"/>
+      <c r="D28" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="37" t="s">
+        <v>154</v>
+      </c>
       <c r="F28" s="38"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>13</v>
       </c>
-      <c r="B29" s="35"/>
+      <c r="B29" s="35" t="s">
+        <v>43</v>
+      </c>
       <c r="C29" s="4"/>
-      <c r="D29" s="39"/>
-      <c r="E29" s="37"/>
+      <c r="D29" s="39" t="s">
+        <v>153</v>
+      </c>
+      <c r="E29" s="37" t="s">
+        <v>154</v>
+      </c>
       <c r="F29" s="38"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>14</v>
       </c>
-      <c r="B30" s="35"/>
+      <c r="B30" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="C30" s="4"/>
-      <c r="D30" s="39"/>
-      <c r="E30" s="37"/>
+      <c r="D30" s="39" t="s">
+        <v>156</v>
+      </c>
+      <c r="E30" s="37" t="s">
+        <v>154</v>
+      </c>
       <c r="F30" s="38"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>15</v>
       </c>
-      <c r="B31" s="35"/>
+      <c r="B31" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="C31" s="4"/>
-      <c r="D31" s="39"/>
-      <c r="E31" s="37"/>
+      <c r="D31" s="39" t="s">
+        <v>155</v>
+      </c>
+      <c r="E31" s="37" t="s">
+        <v>154</v>
+      </c>
       <c r="F31" s="38"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>16</v>
       </c>
-      <c r="B32" s="35"/>
+      <c r="B32" s="35" t="s">
+        <v>46</v>
+      </c>
       <c r="C32" s="4"/>
-      <c r="D32" s="39"/>
-      <c r="E32" s="37"/>
+      <c r="D32" s="39" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="37" t="s">
+        <v>154</v>
+      </c>
       <c r="F32" s="38"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.35">

</xml_diff>